<commit_message>
Changing underlying storage to any `PinnedVec`
* Instead of hard-coded `SplitVec`, the concurrent bag now wraps any `PinnedVec`.
* `capacity` method is added.
* `Debug` is implemented.
* Benchmarks added and reported.
</commit_message>
<xml_diff>
--- a/benches/results/grow.xlsx
+++ b/benches/results/grow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\uurdev\orx\orx-concurrent-bag\benches\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F637EAC6-BB2C-4EA4-AB3A-4D9248B792D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1725B2-3870-44B1-89F8-DC80E8977E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{201707E4-C870-4993-88CE-4A7BD9846E2B}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{201707E4-C870-4993-88CE-4A7BD9846E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="growth" sheetId="5" r:id="rId1"/>
@@ -36,21 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>number of elements</t>
-  </si>
-  <si>
-    <t>ConcurrentBag</t>
   </si>
   <si>
     <t>rayon</t>
   </si>
   <si>
     <t>workload</t>
-  </si>
-  <si>
-    <t>20ms</t>
   </si>
   <si>
     <t>output size: i32</t>
@@ -67,11 +61,23 @@
 output size: [i32; 32]</t>
   </si>
   <si>
-    <t>parallelization</t>
+    <t>number of elements
+per thread</t>
   </si>
   <si>
-    <t>number of elements
-per thread</t>
+    <t>ConcurrentBag (FixedVec)</t>
+  </si>
+  <si>
+    <t>ConcurrentBag (SplitVec&lt;_, Doubling&gt;)</t>
+  </si>
+  <si>
+    <t>ConcurrentBag (SplitVec&lt;_, Linear&gt;)</t>
+  </si>
+  <si>
+    <t>20ns</t>
+  </si>
+  <si>
+    <t>method</t>
   </si>
 </sst>
 </file>
@@ -103,7 +109,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,8 +122,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -248,11 +260,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -294,17 +348,44 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,15 +705,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7FC78D-902C-4DF1-8F50-38A3D8921053}">
-  <dimension ref="B1:I25"/>
+  <dimension ref="B1:I41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" customWidth="1"/>
     <col min="3" max="4" width="29.7109375" customWidth="1"/>
     <col min="5" max="8" width="17.7109375" customWidth="1"/>
   </cols>
@@ -642,445 +723,828 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>4096</v>
+        <v>16384</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.75648000000000004</v>
-      </c>
-      <c r="G2">
-        <v>16.989999999999998</v>
-      </c>
-      <c r="I2">
-        <v>6.2013999999999996</v>
+        <v>0.25753999999999999</v>
+      </c>
+      <c r="G2" s="28">
+        <v>17.97</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>4096</v>
+        <v>16384</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>7.5951000000000004</v>
-      </c>
-      <c r="G3">
-        <v>15.91</v>
-      </c>
-      <c r="I3">
-        <v>8.4968000000000004</v>
+        <v>5.31</v>
+      </c>
+      <c r="G3" s="28">
+        <v>10.56</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" t="str">
+      <c r="B4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>16384</v>
+      </c>
+      <c r="D4" s="24">
+        <v>0</v>
+      </c>
+      <c r="E4" s="23">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F4" s="23"/>
+      <c r="G4" s="29">
+        <v>12.49</v>
+      </c>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="25">
+        <v>16384</v>
+      </c>
+      <c r="D5" s="26">
+        <v>0</v>
+      </c>
+      <c r="E5" s="25">
+        <v>3.94</v>
+      </c>
+      <c r="F5" s="25"/>
+      <c r="G5" s="30">
+        <v>10.96</v>
+      </c>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="str">
         <f>B2</f>
         <v>rayon</v>
       </c>
-      <c r="C4">
-        <v>4096</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>140.69</v>
-      </c>
-      <c r="G4">
-        <v>78.98</v>
-      </c>
-      <c r="H4">
-        <v>58.61</v>
-      </c>
-      <c r="I4">
-        <v>155.61000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" t="str">
-        <f t="shared" ref="B5:B9" si="0">B3</f>
-        <v>ConcurrentBag</v>
-      </c>
-      <c r="C5">
-        <v>4096</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>54.811999999999998</v>
-      </c>
-      <c r="G5">
-        <v>58.61</v>
-      </c>
-      <c r="I5">
-        <v>232.21</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" t="str">
+      <c r="C6">
+        <v>16384</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0.5413</v>
+      </c>
+      <c r="G6" s="29">
+        <v>20.305</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="str">
+        <f>B3</f>
+        <v>ConcurrentBag (SplitVec&lt;_, Doubling&gt;)</v>
+      </c>
+      <c r="C7">
+        <v>16384</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="27">
+        <v>5.8747999999999996</v>
+      </c>
+      <c r="G7" s="29">
+        <v>11.11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="str">
+        <f t="shared" ref="B8:B17" si="0">B4</f>
+        <v>ConcurrentBag (SplitVec&lt;_, Linear&gt;)</v>
+      </c>
+      <c r="C8">
+        <v>16384</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="27">
+        <v>5.1985999999999999</v>
+      </c>
+      <c r="G8" s="29">
+        <v>15.121</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>ConcurrentBag (FixedVec)</v>
+      </c>
+      <c r="C9" s="25">
+        <v>16384</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="25">
+        <v>4.3098999999999998</v>
+      </c>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25">
+        <v>14.41</v>
+      </c>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>rayon</v>
       </c>
-      <c r="C6">
-        <v>16384</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C10">
+        <v>65536</v>
+      </c>
+      <c r="D10" s="1">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>1.9319</v>
-      </c>
-      <c r="G6">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" t="str">
+      <c r="E10" s="27">
+        <v>1.3112999999999999</v>
+      </c>
+      <c r="G10" s="28">
+        <v>81.753</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v>ConcurrentBag</v>
-      </c>
-      <c r="C7">
-        <v>16384</v>
-      </c>
-      <c r="D7" s="1">
+        <v>ConcurrentBag (SplitVec&lt;_, Doubling&gt;)</v>
+      </c>
+      <c r="C11">
+        <v>65536</v>
+      </c>
+      <c r="D11" s="1">
         <v>0</v>
       </c>
-      <c r="E7">
-        <v>32.561</v>
-      </c>
-      <c r="G7">
-        <v>60.28</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="str">
+      <c r="E11" s="27">
+        <v>22.379000000000001</v>
+      </c>
+      <c r="G11" s="28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>ConcurrentBag (SplitVec&lt;_, Linear&gt;)</v>
+      </c>
+      <c r="C12" s="23">
+        <v>65536</v>
+      </c>
+      <c r="D12" s="24">
+        <v>0</v>
+      </c>
+      <c r="E12" s="27">
+        <v>23.736000000000001</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="G12" s="29">
+        <v>57.13</v>
+      </c>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>ConcurrentBag (FixedVec)</v>
+      </c>
+      <c r="C13" s="25">
+        <v>65536</v>
+      </c>
+      <c r="D13" s="26">
+        <v>0</v>
+      </c>
+      <c r="E13" s="25">
+        <v>21.577999999999999</v>
+      </c>
+      <c r="F13" s="25"/>
+      <c r="G13" s="30">
+        <v>41.61</v>
+      </c>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>rayon</v>
       </c>
-      <c r="C8">
-        <v>16384</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8">
-        <v>143.53</v>
-      </c>
-      <c r="G8">
-        <v>202.12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" t="str">
+      <c r="C14">
+        <v>65536</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="27">
+        <v>1.3946000000000001</v>
+      </c>
+      <c r="G14" s="29">
+        <v>80.56</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v>ConcurrentBag</v>
-      </c>
-      <c r="C9">
-        <v>16384</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>58.064</v>
-      </c>
-      <c r="G9">
-        <v>74.171999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I12">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:8" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="13" t="str">
+        <v>ConcurrentBag (SplitVec&lt;_, Doubling&gt;)</v>
+      </c>
+      <c r="C15">
+        <v>65536</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="27">
+        <v>22.138999999999999</v>
+      </c>
+      <c r="G15" s="29">
+        <v>52.012</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>ConcurrentBag (SplitVec&lt;_, Linear&gt;)</v>
+      </c>
+      <c r="C16" s="23">
+        <v>65536</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="27">
+        <v>17.111000000000001</v>
+      </c>
+      <c r="F16" s="23"/>
+      <c r="G16" s="29">
+        <v>60.11</v>
+      </c>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>ConcurrentBag (FixedVec)</v>
+      </c>
+      <c r="C17" s="25">
+        <v>65536</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="25">
+        <v>19.364999999999998</v>
+      </c>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25">
+        <v>52.118000000000002</v>
+      </c>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+    </row>
+    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="13" t="str">
         <f>D1</f>
         <v>workload</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="str">
+      <c r="E25" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="16"/>
+      <c r="G25" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="17"/>
+    </row>
+    <row r="26" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="str">
         <f>B2</f>
         <v>rayon</v>
       </c>
-      <c r="C18" s="2">
-        <f>C2</f>
-        <v>4096</v>
-      </c>
-      <c r="D18" s="10">
-        <f t="shared" ref="D18:D25" si="1">D2</f>
+      <c r="C26" s="2">
+        <f t="shared" ref="C26:C41" si="1">C2</f>
+        <v>16384</v>
+      </c>
+      <c r="D26" s="10">
+        <f t="shared" ref="B26:D26" si="2">D2</f>
         <v>0</v>
       </c>
-      <c r="E18" s="8">
-        <f>E2</f>
-        <v>0.75648000000000004</v>
-      </c>
-      <c r="F18" s="5">
-        <f>E18/E$18</f>
+      <c r="E26" s="8">
+        <f t="shared" ref="E26:E41" si="3">E2</f>
+        <v>0.25753999999999999</v>
+      </c>
+      <c r="F26" s="5">
+        <f>E26/E$26</f>
         <v>1</v>
       </c>
-      <c r="G18" s="8">
-        <f>G2</f>
-        <v>16.989999999999998</v>
-      </c>
-      <c r="H18" s="5">
-        <f>G18/G$18</f>
+      <c r="G26" s="8">
+        <f t="shared" ref="G26:G41" si="4">G2</f>
+        <v>17.97</v>
+      </c>
+      <c r="H26" s="5">
+        <f>G26/G$26</f>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="str">
-        <f>B3</f>
-        <v>ConcurrentBag</v>
-      </c>
-      <c r="C19" s="3">
-        <f>C3</f>
-        <v>4096</v>
-      </c>
-      <c r="D19" s="11">
+    <row r="27" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="18" t="str">
+        <f t="shared" ref="B27:B41" si="5">B3</f>
+        <v>ConcurrentBag (SplitVec&lt;_, Doubling&gt;)</v>
+      </c>
+      <c r="C27" s="19">
         <f t="shared" si="1"/>
+        <v>16384</v>
+      </c>
+      <c r="D27" s="20">
+        <f t="shared" ref="D27:D41" si="6">D3</f>
         <v>0</v>
       </c>
-      <c r="E19" s="9">
-        <f>E3</f>
-        <v>7.5951000000000004</v>
-      </c>
-      <c r="F19" s="7">
-        <f>E19/E$18</f>
-        <v>10.040053934010153</v>
-      </c>
-      <c r="G19" s="9">
-        <f>G3</f>
-        <v>15.91</v>
-      </c>
-      <c r="H19" s="7">
-        <f>G19/G$18</f>
-        <v>0.93643319599764574</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="str">
-        <f>B4</f>
+      <c r="E27" s="21">
+        <f t="shared" si="3"/>
+        <v>5.31</v>
+      </c>
+      <c r="F27" s="22">
+        <f t="shared" ref="F27:F29" si="7">E27/E$26</f>
+        <v>20.618156402888872</v>
+      </c>
+      <c r="G27" s="21">
+        <f t="shared" si="4"/>
+        <v>10.56</v>
+      </c>
+      <c r="H27" s="22">
+        <f t="shared" ref="H27:H29" si="8">G27/G$26</f>
+        <v>0.58764607679465786</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>ConcurrentBag (SplitVec&lt;_, Linear&gt;)</v>
+      </c>
+      <c r="C28" s="19">
+        <f t="shared" si="1"/>
+        <v>16384</v>
+      </c>
+      <c r="D28" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="21">
+        <f t="shared" si="3"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F28" s="22">
+        <f t="shared" si="7"/>
+        <v>19.802749087520386</v>
+      </c>
+      <c r="G28" s="21">
+        <f t="shared" si="4"/>
+        <v>12.49</v>
+      </c>
+      <c r="H28" s="22">
+        <f t="shared" si="8"/>
+        <v>0.69504730105731782</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>ConcurrentBag (FixedVec)</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="1"/>
+        <v>16384</v>
+      </c>
+      <c r="D29" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="9">
+        <f t="shared" si="3"/>
+        <v>3.94</v>
+      </c>
+      <c r="F29" s="7">
+        <f t="shared" si="7"/>
+        <v>15.298594393103985</v>
+      </c>
+      <c r="G29" s="9">
+        <f t="shared" si="4"/>
+        <v>10.96</v>
+      </c>
+      <c r="H29" s="7">
+        <f t="shared" si="8"/>
+        <v>0.60990539788536458</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="str">
+        <f t="shared" si="5"/>
         <v>rayon</v>
       </c>
-      <c r="C20" s="2">
-        <f>C4</f>
-        <v>4096</v>
-      </c>
-      <c r="D20" s="10" t="str">
+      <c r="C30" s="2">
         <f t="shared" si="1"/>
-        <v>20ms</v>
-      </c>
-      <c r="E20" s="8">
-        <f>E4</f>
-        <v>140.69</v>
-      </c>
-      <c r="F20" s="5">
-        <f>E20/E$20</f>
+        <v>16384</v>
+      </c>
+      <c r="D30" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v>20ns</v>
+      </c>
+      <c r="E30" s="8">
+        <f t="shared" si="3"/>
+        <v>0.5413</v>
+      </c>
+      <c r="F30" s="5">
+        <f>E30/E$30</f>
         <v>1</v>
       </c>
-      <c r="G20" s="8">
-        <f>G4</f>
-        <v>78.98</v>
-      </c>
-      <c r="H20" s="5">
-        <f>G20/G$20</f>
+      <c r="G30" s="8">
+        <f t="shared" si="4"/>
+        <v>20.305</v>
+      </c>
+      <c r="H30" s="5">
+        <f>G30/G$30</f>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="str">
-        <f>B5</f>
-        <v>ConcurrentBag</v>
-      </c>
-      <c r="C21" s="3">
-        <f>C5</f>
-        <v>4096</v>
-      </c>
-      <c r="D21" s="11" t="str">
+    <row r="31" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>ConcurrentBag (SplitVec&lt;_, Doubling&gt;)</v>
+      </c>
+      <c r="C31" s="19">
         <f t="shared" si="1"/>
-        <v>20ms</v>
-      </c>
-      <c r="E21" s="9">
-        <f>E5</f>
-        <v>54.811999999999998</v>
-      </c>
-      <c r="F21" s="7">
-        <f>E21/E$20</f>
-        <v>0.3895941431516099</v>
-      </c>
-      <c r="G21" s="9">
-        <f>G5</f>
-        <v>58.61</v>
-      </c>
-      <c r="H21" s="7">
-        <f>G21/G$20</f>
-        <v>0.74208660420359585</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="str">
-        <f>B6</f>
+        <v>16384</v>
+      </c>
+      <c r="D31" s="20" t="str">
+        <f t="shared" si="6"/>
+        <v>20ns</v>
+      </c>
+      <c r="E31" s="21">
+        <f t="shared" si="3"/>
+        <v>5.8747999999999996</v>
+      </c>
+      <c r="F31" s="22">
+        <f t="shared" ref="F31:F33" si="9">E31/E$30</f>
+        <v>10.853131350452614</v>
+      </c>
+      <c r="G31" s="21">
+        <f t="shared" si="4"/>
+        <v>11.11</v>
+      </c>
+      <c r="H31" s="22">
+        <f t="shared" ref="H31:H33" si="10">G31/G$30</f>
+        <v>0.54715587293770007</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>ConcurrentBag (SplitVec&lt;_, Linear&gt;)</v>
+      </c>
+      <c r="C32" s="19">
+        <f t="shared" si="1"/>
+        <v>16384</v>
+      </c>
+      <c r="D32" s="20" t="str">
+        <f t="shared" si="6"/>
+        <v>20ns</v>
+      </c>
+      <c r="E32" s="21">
+        <f t="shared" si="3"/>
+        <v>5.1985999999999999</v>
+      </c>
+      <c r="F32" s="22">
+        <f t="shared" si="9"/>
+        <v>9.6039164973212632</v>
+      </c>
+      <c r="G32" s="21">
+        <f t="shared" si="4"/>
+        <v>15.121</v>
+      </c>
+      <c r="H32" s="22">
+        <f t="shared" si="10"/>
+        <v>0.74469342526471316</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>ConcurrentBag (FixedVec)</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="1"/>
+        <v>16384</v>
+      </c>
+      <c r="D33" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>20ns</v>
+      </c>
+      <c r="E33" s="9">
+        <f t="shared" si="3"/>
+        <v>4.3098999999999998</v>
+      </c>
+      <c r="F33" s="7">
+        <f t="shared" si="9"/>
+        <v>7.9621282098651394</v>
+      </c>
+      <c r="G33" s="9">
+        <f t="shared" si="4"/>
+        <v>14.41</v>
+      </c>
+      <c r="H33" s="7">
+        <f t="shared" si="10"/>
+        <v>0.70967741935483875</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="str">
+        <f t="shared" si="5"/>
         <v>rayon</v>
       </c>
-      <c r="C22" s="2">
-        <f>C6</f>
-        <v>16384</v>
-      </c>
-      <c r="D22" s="10">
+      <c r="C34" s="2">
         <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="D34" s="10">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E22" s="8">
-        <f>E6</f>
-        <v>1.9319</v>
-      </c>
-      <c r="F22" s="5">
-        <f>E22/E$22</f>
+      <c r="E34" s="8">
+        <f t="shared" si="3"/>
+        <v>1.3112999999999999</v>
+      </c>
+      <c r="F34" s="5">
+        <f>E34/E$34</f>
         <v>1</v>
       </c>
-      <c r="G22" s="8">
-        <f>G6</f>
-        <v>156</v>
-      </c>
-      <c r="H22" s="5">
-        <f>G22/G$22</f>
+      <c r="G34" s="8">
+        <f t="shared" si="4"/>
+        <v>81.753</v>
+      </c>
+      <c r="H34" s="5">
+        <f>G34/G$34</f>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="6" t="str">
-        <f>B7</f>
-        <v>ConcurrentBag</v>
-      </c>
-      <c r="C23" s="3">
-        <f>C7</f>
-        <v>16384</v>
-      </c>
-      <c r="D23" s="11">
+    <row r="35" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>ConcurrentBag (SplitVec&lt;_, Doubling&gt;)</v>
+      </c>
+      <c r="C35" s="19">
         <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="D35" s="20">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E23" s="9">
-        <f>E7</f>
-        <v>32.561</v>
-      </c>
-      <c r="F23" s="7">
-        <f>E23/E$22</f>
-        <v>16.854392049277912</v>
-      </c>
-      <c r="G23" s="9">
-        <f>G7</f>
-        <v>60.28</v>
-      </c>
-      <c r="H23" s="7">
-        <f>G23/G$22</f>
-        <v>0.38641025641025639</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="str">
-        <f>B8</f>
+      <c r="E35" s="21">
+        <f t="shared" si="3"/>
+        <v>22.379000000000001</v>
+      </c>
+      <c r="F35" s="22">
+        <f t="shared" ref="F35:F37" si="11">E35/E$34</f>
+        <v>17.066270113627699</v>
+      </c>
+      <c r="G35" s="21">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="H35" s="22">
+        <f t="shared" ref="H35:H37" si="12">G35/G$34</f>
+        <v>0.61159835113084537</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>ConcurrentBag (SplitVec&lt;_, Linear&gt;)</v>
+      </c>
+      <c r="C36" s="19">
+        <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="D36" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="21">
+        <f t="shared" si="3"/>
+        <v>23.736000000000001</v>
+      </c>
+      <c r="F36" s="22">
+        <f t="shared" si="11"/>
+        <v>18.101121024937086</v>
+      </c>
+      <c r="G36" s="21">
+        <f t="shared" si="4"/>
+        <v>57.13</v>
+      </c>
+      <c r="H36" s="22">
+        <f t="shared" si="12"/>
+        <v>0.69881227600210394</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>ConcurrentBag (FixedVec)</v>
+      </c>
+      <c r="C37" s="3">
+        <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="D37" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E37" s="9">
+        <f t="shared" si="3"/>
+        <v>21.577999999999999</v>
+      </c>
+      <c r="F37" s="7">
+        <f t="shared" si="11"/>
+        <v>16.455425913215894</v>
+      </c>
+      <c r="G37" s="9">
+        <f t="shared" si="4"/>
+        <v>41.61</v>
+      </c>
+      <c r="H37" s="7">
+        <f t="shared" si="12"/>
+        <v>0.50897214781108946</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="str">
+        <f t="shared" si="5"/>
         <v>rayon</v>
       </c>
-      <c r="C24" s="2">
-        <f>C8</f>
-        <v>16384</v>
-      </c>
-      <c r="D24" s="10" t="str">
+      <c r="C38" s="2">
         <f t="shared" si="1"/>
-        <v>20ms</v>
-      </c>
-      <c r="E24" s="8">
-        <f>E8</f>
-        <v>143.53</v>
-      </c>
-      <c r="F24" s="5">
-        <f>E24/E$24</f>
+        <v>65536</v>
+      </c>
+      <c r="D38" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v>20ns</v>
+      </c>
+      <c r="E38" s="8">
+        <f t="shared" si="3"/>
+        <v>1.3946000000000001</v>
+      </c>
+      <c r="F38" s="5">
+        <f>E38/E$38</f>
         <v>1</v>
       </c>
-      <c r="G24" s="8">
-        <f>G8</f>
-        <v>202.12</v>
-      </c>
-      <c r="H24" s="5">
-        <f>G24/G$24</f>
+      <c r="G38" s="8">
+        <f t="shared" si="4"/>
+        <v>80.56</v>
+      </c>
+      <c r="H38" s="5">
+        <f>G38/G$38</f>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="str">
-        <f>B9</f>
-        <v>ConcurrentBag</v>
-      </c>
-      <c r="C25" s="3">
-        <f>C9</f>
-        <v>16384</v>
-      </c>
-      <c r="D25" s="11" t="str">
+    <row r="39" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>ConcurrentBag (SplitVec&lt;_, Doubling&gt;)</v>
+      </c>
+      <c r="C39" s="19">
         <f t="shared" si="1"/>
-        <v>20ms</v>
-      </c>
-      <c r="E25" s="9">
-        <f>E9</f>
-        <v>58.064</v>
-      </c>
-      <c r="F25" s="7">
-        <f>E25/E$24</f>
-        <v>0.4045426043335888</v>
-      </c>
-      <c r="G25" s="9">
-        <f>G9</f>
-        <v>74.171999999999997</v>
-      </c>
-      <c r="H25" s="7">
-        <f>G25/G$24</f>
-        <v>0.36697011676231939</v>
+        <v>65536</v>
+      </c>
+      <c r="D39" s="20" t="str">
+        <f t="shared" si="6"/>
+        <v>20ns</v>
+      </c>
+      <c r="E39" s="21">
+        <f t="shared" si="3"/>
+        <v>22.138999999999999</v>
+      </c>
+      <c r="F39" s="22">
+        <f t="shared" ref="F39:F41" si="13">E39/E$38</f>
+        <v>15.874802810841818</v>
+      </c>
+      <c r="G39" s="21">
+        <f t="shared" si="4"/>
+        <v>52.012</v>
+      </c>
+      <c r="H39" s="22">
+        <f t="shared" ref="H39:H41" si="14">G39/G$38</f>
+        <v>0.64563058589870903</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>ConcurrentBag (SplitVec&lt;_, Linear&gt;)</v>
+      </c>
+      <c r="C40" s="19">
+        <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="D40" s="20" t="str">
+        <f t="shared" si="6"/>
+        <v>20ns</v>
+      </c>
+      <c r="E40" s="21">
+        <f t="shared" si="3"/>
+        <v>17.111000000000001</v>
+      </c>
+      <c r="F40" s="22">
+        <f t="shared" si="13"/>
+        <v>12.269467947798653</v>
+      </c>
+      <c r="G40" s="21">
+        <f t="shared" si="4"/>
+        <v>60.11</v>
+      </c>
+      <c r="H40" s="22">
+        <f t="shared" si="14"/>
+        <v>0.74615193644488575</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>ConcurrentBag (FixedVec)</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="D41" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>20ns</v>
+      </c>
+      <c r="E41" s="9">
+        <f t="shared" si="3"/>
+        <v>19.364999999999998</v>
+      </c>
+      <c r="F41" s="7">
+        <f t="shared" si="13"/>
+        <v>13.885701993403124</v>
+      </c>
+      <c r="G41" s="9">
+        <f t="shared" si="4"/>
+        <v>52.118000000000002</v>
+      </c>
+      <c r="H41" s="7">
+        <f t="shared" si="14"/>
+        <v>0.6469463753723933</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
   </mergeCells>
-  <conditionalFormatting sqref="F18:F19">
+  <conditionalFormatting sqref="F26:F29">
     <cfRule type="dataBar" priority="8">
       <dataBar showValue="0">
         <cfvo type="min"/>
@@ -1094,7 +1558,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F21">
+  <conditionalFormatting sqref="F30:F33">
     <cfRule type="dataBar" priority="7">
       <dataBar showValue="0">
         <cfvo type="min"/>
@@ -1108,7 +1572,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F23">
+  <conditionalFormatting sqref="F34:F37">
     <cfRule type="dataBar" priority="6">
       <dataBar showValue="0">
         <cfvo type="min"/>
@@ -1122,7 +1586,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F24:F25">
+  <conditionalFormatting sqref="F38:F41">
     <cfRule type="dataBar" priority="5">
       <dataBar showValue="0">
         <cfvo type="min"/>
@@ -1136,7 +1600,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18:H19">
+  <conditionalFormatting sqref="H26:H29">
     <cfRule type="dataBar" priority="4">
       <dataBar showValue="0">
         <cfvo type="min"/>
@@ -1150,7 +1614,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20:H21">
+  <conditionalFormatting sqref="H30:H33">
     <cfRule type="dataBar" priority="3">
       <dataBar showValue="0">
         <cfvo type="min"/>
@@ -1164,7 +1628,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22:H23">
+  <conditionalFormatting sqref="H34:H37">
     <cfRule type="dataBar" priority="2">
       <dataBar showValue="0">
         <cfvo type="min"/>
@@ -1178,7 +1642,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24:H25">
+  <conditionalFormatting sqref="H38:H41">
     <cfRule type="dataBar" priority="1">
       <dataBar showValue="0">
         <cfvo type="min"/>
@@ -1194,9 +1658,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="F18:F25 G18:G25" formula="1"/>
-  </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -1209,7 +1670,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F18:F19</xm:sqref>
+          <xm:sqref>F26:F29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4B8F1DF9-AF92-48B3-92F1-001448B4A017}">
@@ -1220,7 +1681,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F20:F21</xm:sqref>
+          <xm:sqref>F30:F33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{21C99A28-1CAC-4B17-A70E-A8D9E6030683}">
@@ -1231,7 +1692,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F22:F23</xm:sqref>
+          <xm:sqref>F34:F37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C1542B4F-C815-48F6-8D42-21DA975D34CF}">
@@ -1242,7 +1703,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F24:F25</xm:sqref>
+          <xm:sqref>F38:F41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{627311B3-B6B8-4CCB-B3C2-F1D77A962B62}">
@@ -1253,7 +1714,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H18:H19</xm:sqref>
+          <xm:sqref>H26:H29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{3D1EF6E5-53F3-4100-ABDC-DDFE5F43B8F4}">
@@ -1264,7 +1725,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H20:H21</xm:sqref>
+          <xm:sqref>H30:H33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{797CD07D-31EB-4762-BEBB-2FA26E0D1365}">
@@ -1275,7 +1736,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H22:H23</xm:sqref>
+          <xm:sqref>H34:H37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{ECB5298B-030E-4B3D-9008-3CAFAC2EA877}">
@@ -1286,7 +1747,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H24:H25</xm:sqref>
+          <xm:sqref>H38:H41</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>